<commit_message>
Major update of KoreanPOSTagger and DependencyParser
</commit_message>
<xml_diff>
--- a/data/ko/pos/ko-pos-dic.xlsx
+++ b/data/ko/pos/ko-pos-dic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="eomi" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="188">
   <si>
     <t>었</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>지만/EC</t>
-  </si>
-  <si>
-    <t>라/EFO</t>
   </si>
   <si>
     <t>느려서</t>
@@ -523,9 +520,6 @@
     <t>다/JX</t>
   </si>
   <si>
-    <t>ㄷ</t>
-  </si>
-  <si>
     <t>데다</t>
   </si>
   <si>
@@ -596,6 +590,18 @@
   </si>
   <si>
     <t>되/XSV</t>
+  </si>
+  <si>
+    <t>ㅂ니까</t>
+  </si>
+  <si>
+    <t>ㅂ니까/EF</t>
+  </si>
+  <si>
+    <t>라/EF</t>
+  </si>
+  <si>
+    <t>-워</t>
   </si>
 </sst>
 </file>
@@ -671,8 +677,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -820,7 +840,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="149">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -888,6 +908,13 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -955,6 +982,13 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1284,11 +1318,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1307,19 +1341,19 @@
         <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>36</v>
@@ -1361,7 +1395,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1369,19 +1403,19 @@
         <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1389,13 +1423,16 @@
         <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1403,10 +1440,10 @@
         <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1414,19 +1451,19 @@
         <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="G8" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1434,10 +1471,10 @@
         <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1478,14 +1515,14 @@
         <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1493,16 +1530,16 @@
         <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="G14" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1538,7 +1575,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
@@ -1559,7 +1596,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
@@ -1577,7 +1614,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1585,10 +1622,10 @@
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1618,10 +1655,10 @@
         <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1629,10 +1666,10 @@
         <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1640,17 +1677,17 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1669,13 +1706,13 @@
         <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1700,7 +1737,7 @@
         <v>9</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1730,20 +1767,20 @@
         <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G32" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1784,16 +1821,16 @@
         <v>38</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1801,16 +1838,16 @@
         <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1818,13 +1855,13 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1832,13 +1869,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1846,14 +1883,14 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>43</v>
@@ -1864,17 +1901,17 @@
         <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1882,17 +1919,28 @@
         <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1913,9 +1961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1932,19 +1980,19 @@
         <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>36</v>
@@ -1955,242 +2003,242 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>161</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2211,9 +2259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2231,19 +2279,19 @@
         <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>36</v>
@@ -2254,170 +2302,170 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>46</v>
@@ -2425,46 +2473,46 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major update of Korean morpheme analyzer. This is temporary commit.
</commit_message>
<xml_diff>
--- a/data/ko/pos/ko-pos-dic.xlsx
+++ b/data/ko/pos/ko-pos-dic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="eomi" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="228">
   <si>
     <t>었</t>
   </si>
@@ -179,9 +179,6 @@
     <t>ㅕ서</t>
   </si>
   <si>
-    <t>ㅆ다</t>
-  </si>
-  <si>
     <t>봐</t>
   </si>
   <si>
@@ -426,9 +423,6 @@
   </si>
   <si>
     <t>힘든, 만든</t>
-  </si>
-  <si>
-    <t>만들기</t>
   </si>
   <si>
     <t>갔다</t>
@@ -517,9 +511,6 @@
     <t>으</t>
   </si>
   <si>
-    <t>다/JX</t>
-  </si>
-  <si>
     <t>데다</t>
   </si>
   <si>
@@ -602,6 +593,135 @@
   </si>
   <si>
     <t>-워</t>
+  </si>
+  <si>
+    <t>음운(phoneme)제약조건</t>
+  </si>
+  <si>
+    <t>#음절(surface)</t>
+  </si>
+  <si>
+    <t>형태(morpheme)제약조건</t>
+  </si>
+  <si>
+    <t>품사(pos)제약조건</t>
+  </si>
+  <si>
+    <t>불규칙(irregular)조건</t>
+  </si>
+  <si>
+    <t>형태소/POS(morpheme)</t>
+  </si>
+  <si>
+    <t>습니다</t>
+  </si>
+  <si>
+    <t>습니다/EF</t>
+  </si>
+  <si>
+    <t>하</t>
+  </si>
+  <si>
+    <t>하/XSV</t>
+  </si>
+  <si>
+    <t>과</t>
+  </si>
+  <si>
+    <t>과/JC</t>
+  </si>
+  <si>
+    <t>으나</t>
+  </si>
+  <si>
+    <t>으나/EC</t>
+  </si>
+  <si>
+    <t>와</t>
+  </si>
+  <si>
+    <t>와/JC</t>
+  </si>
+  <si>
+    <t>적/VCP</t>
+  </si>
+  <si>
+    <t>에서</t>
+  </si>
+  <si>
+    <t>에서/JKB</t>
+  </si>
+  <si>
+    <t>냐는</t>
+  </si>
+  <si>
+    <t>냐는/ETM</t>
+  </si>
+  <si>
+    <t>로</t>
+  </si>
+  <si>
+    <t>로/JKB</t>
+  </si>
+  <si>
+    <t>#ㅆ다</t>
+  </si>
+  <si>
+    <t>데다/JX</t>
+  </si>
+  <si>
+    <t>어</t>
+  </si>
+  <si>
+    <t>어/EC</t>
+  </si>
+  <si>
+    <t>엔</t>
+  </si>
+  <si>
+    <t>에/JKB+는/JX</t>
+  </si>
+  <si>
+    <t>으로써</t>
+  </si>
+  <si>
+    <t>으로써/JKB</t>
+  </si>
+  <si>
+    <t>ㅁ</t>
+  </si>
+  <si>
+    <t>ㅁ/ETN</t>
+  </si>
+  <si>
+    <t>함으로써</t>
+  </si>
+  <si>
+    <t>함께</t>
+  </si>
+  <si>
+    <t>함께/MAG</t>
+  </si>
+  <si>
+    <t>부사</t>
+  </si>
+  <si>
+    <t>~와 함께</t>
+  </si>
+  <si>
+    <t>와/JKB</t>
+  </si>
+  <si>
+    <t>과/JKB</t>
+  </si>
+  <si>
+    <t>~과 함께</t>
+  </si>
+  <si>
+    <t>내</t>
+  </si>
+  <si>
+    <t>내/VX</t>
   </si>
 </sst>
 </file>
@@ -677,8 +797,92 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="149">
+  <cellStyleXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -840,7 +1044,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="149">
+  <cellStyles count="233">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -915,6 +1119,48 @@
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -989,6 +1235,48 @@
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1318,20 +1606,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="22.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="1" customWidth="1"/>
-    <col min="6" max="7" width="13.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="31.83203125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -1341,22 +1631,22 @@
         <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>186</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>35</v>
+        <v>190</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>188</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>189</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>39</v>
@@ -1367,10 +1657,17 @@
         <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>110</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1378,10 +1675,10 @@
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1394,28 +1691,25 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1423,16 +1717,16 @@
         <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1440,10 +1734,10 @@
         <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1451,19 +1745,19 @@
         <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1471,10 +1765,10 @@
         <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1482,10 +1776,10 @@
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>204</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1493,10 +1787,10 @@
         <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1504,10 +1798,10 @@
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1515,14 +1809,10 @@
         <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="1" t="s">
-        <v>150</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1530,16 +1820,14 @@
         <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>133</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="1" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1547,10 +1835,16 @@
         <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>131</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1558,10 +1852,10 @@
         <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1569,20 +1863,10 @@
         <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1590,20 +1874,20 @@
         <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1611,10 +1895,20 @@
         <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>186</v>
+        <v>15</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1622,10 +1916,10 @@
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1633,10 +1927,10 @@
         <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>159</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1644,10 +1938,10 @@
         <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1655,10 +1949,13 @@
         <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>165</v>
+        <v>217</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1666,10 +1963,10 @@
         <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>143</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>144</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1677,17 +1974,10 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>163</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1695,10 +1985,10 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>181</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>4</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1706,13 +1996,10 @@
         <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1720,10 +2007,10 @@
         <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>33</v>
+        <v>191</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>15</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1731,13 +2018,10 @@
         <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>119</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1745,10 +2029,13 @@
         <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>6</v>
+        <v>147</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1756,10 +2043,10 @@
         <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1767,20 +2054,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>115</v>
+        <v>210</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>117</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1788,10 +2065,13 @@
         <v>38</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1799,10 +2079,10 @@
         <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1810,10 +2090,10 @@
         <v>38</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1821,16 +2101,20 @@
         <v>38</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G36" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1838,16 +2122,10 @@
         <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>124</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1855,13 +2133,10 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>170</v>
+        <v>20</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>171</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1869,13 +2144,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>154</v>
+        <v>28</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>156</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1883,17 +2155,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1901,17 +2166,16 @@
         <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="3"/>
+        <v>4</v>
+      </c>
       <c r="G41" s="3" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1919,17 +2183,16 @@
         <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F42" s="3"/>
+        <v>15</v>
+      </c>
       <c r="G42" s="3" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1937,14 +2200,85 @@
         <v>38</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>185</v>
+        <v>9</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H42">
+  <sortState ref="A2:H48">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1959,11 +2293,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1980,19 +2314,19 @@
         <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>36</v>
@@ -2003,134 +2337,137 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>195</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>195</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>159</v>
+        <v>224</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>160</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>84</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>209</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>206</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>99</v>
@@ -2141,108 +2478,188 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:H22">
+  <sortState ref="A2:H29">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2257,11 +2674,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2279,19 +2696,19 @@
         <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>36</v>
@@ -2302,79 +2719,79 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>167</v>
+        <v>226</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>168</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>109</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>179</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>128</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>176</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2382,142 +2799,208 @@
         <v>105</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>178</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>173</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>153</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>176</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>177</v>
+        <v>90</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
+      <c r="B23" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>114</v>
+      <c r="C25" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H20">
-    <sortCondition ref="C2"/>
+  <sortState ref="A2:H26">
+    <sortCondition ref="C17"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Major updates of named entity recognizer, dependency parser because of updates of Korean POS tagger
</commit_message>
<xml_diff>
--- a/data/ko/pos/ko-pos-dic.xlsx
+++ b/data/ko/pos/ko-pos-dic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="0" windowWidth="26120" windowHeight="13660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="eomi" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="954">
   <si>
     <t>었</t>
   </si>
@@ -2924,6 +2924,9 @@
   <si>
     <t>+ㄴ -는</t>
   </si>
+  <si>
+    <t>#만</t>
+  </si>
 </sst>
 </file>
 
@@ -2935,7 +2938,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3040,8 +3043,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1957">
+  <cellStyleXfs count="1959">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5026,7 +5031,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1957">
+  <cellStyles count="1959">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -6005,6 +6010,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1952" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1954" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1956" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1958" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6983,6 +6989,7 @@
     <cellStyle name="Hyperlink" xfId="1951" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1953" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1955" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1957" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -11586,7 +11593,7 @@
   <dimension ref="A1:L186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -15815,8 +15822,8 @@
   <dimension ref="A1:L187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16004,7 +16011,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>953</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>436</v>
@@ -16016,7 +16023,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
-        <v>78</v>
+        <v>953</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>434</v>

</xml_diff>